<commit_message>
modificacion de datos de hospitales
2014 OK - falta revisar isla de pascua y los demas años
</commit_message>
<xml_diff>
--- a/Memoria/data/Hospitales_restantes.xlsx
+++ b/Memoria/data/Hospitales_restantes.xlsx
@@ -8,24 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO T14S\Desktop\Memoria 2\Memoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451ECC8E-96DD-4E58-AF13-ADBB006448BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0216E90-4EDA-4717-850C-E74061BD056A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33285" yWindow="2205" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="1" r:id="rId1"/>
+    <sheet name="2015" sheetId="2" r:id="rId2"/>
+    <sheet name="2016" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Hospital de Alto Hospicio</t>
   </si>
@@ -34,13 +47,112 @@
   </si>
   <si>
     <t>Hospital Metropolitano</t>
+  </si>
+  <si>
+    <t>Centro Asistencial Norte</t>
+  </si>
+  <si>
+    <t>AtenciÃ³n Primaria de Salud</t>
+  </si>
+  <si>
+    <t>Consultorio General Urbano de San Felipe</t>
+  </si>
+  <si>
+    <t>Consultorio General Urbano NÂº 2 de Los Andes</t>
+  </si>
+  <si>
+    <t>Consultorio General Urbano de Llay Llay</t>
+  </si>
+  <si>
+    <t>Consultorio Violeta Parra</t>
+  </si>
+  <si>
+    <t>Centro Comunitario Salud Mental</t>
+  </si>
+  <si>
+    <t>Consultorio VÃ­ctor Manuel FernÃ¡ndez</t>
+  </si>
+  <si>
+    <t>Centro de Sangre y Tejidos</t>
+  </si>
+  <si>
+    <t>CESFAM LIRQUEN</t>
+  </si>
+  <si>
+    <t>Hospital Huepil</t>
+  </si>
+  <si>
+    <t>Consultorio de Miraflores</t>
+  </si>
+  <si>
+    <t>Consultorio Externo</t>
+  </si>
+  <si>
+    <t>Consultorio de Hualaihue</t>
+  </si>
+  <si>
+    <t>DirecciÃ³n de Salud Rural</t>
+  </si>
+  <si>
+    <t>Consultorio A. GutiÃ©rrez</t>
+  </si>
+  <si>
+    <t>Consultorio VÃ­ctor Domingo Silva</t>
+  </si>
+  <si>
+    <t>Cecosf Puerto Williams</t>
+  </si>
+  <si>
+    <t>SAMU Magallanes</t>
+  </si>
+  <si>
+    <t>Hospital PsiquiÃ¡trico</t>
+  </si>
+  <si>
+    <t>UNIDAD SALUD MENTAL - CTAS COMPLEMENTARIAS</t>
+  </si>
+  <si>
+    <t>ESTABLECIMIENTO LARGA ESTADIA ADULTO MAYOR</t>
+  </si>
+  <si>
+    <t>DirecciÃ³n AtenciÃ³n Primaria</t>
+  </si>
+  <si>
+    <t>Hospital De Urgencia Asistencia PÃºblica</t>
+  </si>
+  <si>
+    <t>Centro De DiagnÃ³stico TerapÃ©utico</t>
+  </si>
+  <si>
+    <t>Centro de Referencia Salud Occidente Salvador Allende</t>
+  </si>
+  <si>
+    <t>Centro de Referencia de Salud</t>
+  </si>
+  <si>
+    <t>Centro de Referencia de Salud Cordillera PeÃ±alolÃ©n Cordillera Oriente</t>
+  </si>
+  <si>
+    <t>S. SALUD MAGALLANES</t>
+  </si>
+  <si>
+    <t>005 Cecosf Puerto Williams</t>
+  </si>
+  <si>
+    <t>Valdivia</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Hospital de Mariquina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,16 +160,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FFB0B0B0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF323232"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -65,12 +201,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0C1F30"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF0C1F30"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF0C1F30"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF0C1F30"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,45 +559,551 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E5"/>
+  <dimension ref="A3:BV8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>204</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2803</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:74" s="4" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>2206</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
+      <c r="BK6" s="3"/>
+      <c r="BL6" s="3"/>
+      <c r="BM6" s="3"/>
+      <c r="BN6" s="3"/>
+      <c r="BO6" s="3"/>
+      <c r="BP6" s="3"/>
+      <c r="BQ6" s="3"/>
+      <c r="BR6" s="3"/>
+      <c r="BS6" s="3"/>
+      <c r="BT6" s="3"/>
+      <c r="BU6" s="3"/>
+      <c r="BV6" s="3"/>
+    </row>
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="9">
+        <v>122200</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5E389D-4EA9-4FF2-A934-D3409823DF4F}">
+  <dimension ref="A3:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
         <v>204</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C533523D-E9AD-46A7-8505-8EBFCCE317FC}">
+  <dimension ref="A2:D33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>204</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>308</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
+        <v>608</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>808</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>809</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>8010</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>11010</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>11011</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1209</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>12010</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1306</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1403</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1703</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>18010</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
         <v>2004</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>20012</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>2103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>2109</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>21010</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>2206</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>2207</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>2208</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>2209</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>22010</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>22011</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>2403</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>2405</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>2603</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>2703</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
         <v>2803</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D31" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>2804</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>3201</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificación data y graficas
</commit_message>
<xml_diff>
--- a/Memoria/data/Hospitales_restantes.xlsx
+++ b/Memoria/data/Hospitales_restantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO T14S\Desktop\Memoria 2\Memoria\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0216E90-4EDA-4717-850C-E74061BD056A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19722D3C-0A0D-4F17-8C31-9C26F136B151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33285" yWindow="2205" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Hospital de Alto Hospicio</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>Hospital de Mariquina</t>
+  </si>
+  <si>
+    <t>Biobío</t>
+  </si>
+  <si>
+    <t>Hospital Comunitario de Santa Bárbara</t>
+  </si>
+  <si>
+    <t>Magallanes</t>
+  </si>
+  <si>
+    <t>Hospital Comunitario Cristina Calderón de Puerto Williams</t>
   </si>
 </sst>
 </file>
@@ -249,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -278,6 +290,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,15 +577,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:BV8"/>
+  <dimension ref="A3:BV10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:74" x14ac:dyDescent="0.25">
@@ -705,6 +724,34 @@
       <c r="C8" s="10"/>
       <c r="D8" s="12"/>
     </row>
+    <row r="9" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="13">
+        <v>8</v>
+      </c>
+      <c r="C9" s="13">
+        <v>120106</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="13">
+        <v>126704</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B7:B8"/>

</xml_diff>